<commit_message>
Review changes implemented for My products
</commit_message>
<xml_diff>
--- a/testData/qa/customerOverview.xlsx
+++ b/testData/qa/customerOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanvi.gupta\Desktop\customerai\testData\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B9E99-44CD-4C29-91C2-89ED4329BF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A86E1C-AD29-4128-9807-D61FEF84A978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
   </bookViews>
@@ -47,10 +47,10 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Credit Cards: Silver, Gold, Platinum &amp; Millennium|Deposit Account|Mortgage Home Loans|Personal Loans|Savings Account|Wealth Management</t>
+    <t>Wealth Management</t>
   </si>
   <si>
-    <t>Wealth Management</t>
+    <t>Credit Cards|Deposit Account|Mortgage Home Loans|Personal Loans|Savings Account|Wealth Management</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +450,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>